<commit_message>
Dumping n number of files
</commit_message>
<xml_diff>
--- a/StudyTracker.xlsx
+++ b/StudyTracker.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VijayBI\GitHubCom\VBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBI\SCM\GitHubCom\VBI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8532" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OnLinuxPlatform" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Complete OS Concepts along with Linux OS hands on.</t>
   </si>
@@ -92,6 +92,10 @@
   </si>
   <si>
     <t>Once Linux OS is completed concentrate on Android Linux Kernel functionalities along with Android Architecture.</t>
+  </si>
+  <si>
+    <t>Webservice automation using "Block Extensible Exchange Protocol" BEEP as trasport protocol
+BEEP is a new Internet Engineering Task Force (IETF) framework for building new protocols. Which promising alternative for HTTP.</t>
   </si>
 </sst>
 </file>
@@ -417,37 +421,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="77.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -466,17 +470,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="123.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="123.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -492,12 +496,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="99.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="99.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -515,22 +519,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -542,51 +546,56 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="95.42578125" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="95.44140625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>